<commit_message>
update value to 66
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas.QICS\TestToroties\tortoise-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C64320-1A1C-4D5F-8644-745CC6D74508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB163BC-3E54-4783-9F3D-9BE0AD09D51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,15 +339,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update value to 77
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas.QICS\TestToroties\tortoise-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB163BC-3E54-4783-9F3D-9BE0AD09D51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFEFA4B-0056-4E5A-B4D6-961E4043025D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,7 +345,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update value to 99
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas.QICS\TestToroties\tortoise-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFEFA4B-0056-4E5A-B4D6-961E4043025D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC3949F-B4C4-4479-BC1F-C83A3EC218F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,7 +345,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>77</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>